<commit_message>
updated backlog with sprint numbers
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t xml:space="preserve">PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -64,46 +64,46 @@
     <t xml:space="preserve">As a user, I want to be asked to verify before a schedule is deleted, so that I do not accidently delete a schedule.</t>
   </si>
   <si>
+    <t xml:space="preserve">H, 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the app to automatically determine the geographical location of buildings that my classes are in based only on the name of the building as provided by the schedule in the TTU registration system, so that I can easily have my schedule generated without research or prior knowledge of where the buildings are.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to be presented with a message the first time I load the app that informs me of the privacy implications of using the app, so that I am aware of how my information is being handled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the app to show me the shortest walking route between classes, so that I can arrive as quickly as possible in the event that I am running late.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to be able to arbitrarily add some other locations to the app and to my schedules, so that I can plan in regular lunch destinations or walks for exercise between classes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the app to intelligently determine when classes for the day are already over and provide the reduced set of directions only to classes which are not yet over, so that I am not encumbered by excess, unnecessary information.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Undecided</t>
   </si>
   <si>
-    <t xml:space="preserve">H, 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to automatically determine the geographical location of buildings that my classes are in based only on the name of the building as provided by the schedule in the TTU registration system, so that I can easily have my schedule generated without research or prior knowledge of where the buildings are.</t>
+    <t xml:space="preserve">M, 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the app to recalculate the shortest path to the next destination in my schedule with the push of a ‘recalculate’ button, in the event that I veer from the original route and require new directions.</t>
   </si>
   <si>
     <t xml:space="preserve">undecided</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be presented with a message the first time I load the app that informs me of the privacy implications of using the app, so that I am aware of how my information is being handled.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to show me the shortest walking route between classes, so that I can arrive as quickly as possible in the event that I am running late.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to arbitrarily add some other locations to the app and to my schedules, so that I can plan in regular lunch destinations or walks for exercise between classes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to intelligently determine when classes for the day are already over and provide the reduced set of directions only to classes which are not yet over, so that I am not encumbered by excess, unnecessary information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M, 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to recalculate the shortest path to the next destination in my schedule with the push of a ‘recalculate’ button, in the event that I veer from the original route and require new directions.</t>
   </si>
   <si>
     <t xml:space="preserve">M, 8</t>
@@ -567,13 +567,13 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.5"/>
@@ -646,11 +646,11 @@
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>11</v>
@@ -667,13 +667,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>11</v>
@@ -687,13 +687,13 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="D11" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>11</v>
@@ -707,13 +707,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>11</v>
@@ -727,13 +727,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>11</v>
@@ -747,13 +747,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>11</v>
@@ -767,10 +767,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>28</v>
@@ -790,7 +790,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>30</v>
@@ -810,7 +810,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>32</v>
@@ -830,7 +830,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>34</v>
@@ -850,7 +850,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>36</v>
@@ -870,7 +870,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>38</v>
@@ -890,7 +890,7 @@
         <v>39</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>40</v>
@@ -913,7 +913,7 @@
         <v>42</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>43</v>
@@ -936,7 +936,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>46</v>
@@ -959,7 +959,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>48</v>
@@ -982,7 +982,7 @@
         <v>49</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>50</v>
@@ -1002,7 +1002,7 @@
         <v>51</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>52</v>
@@ -1022,7 +1022,7 @@
         <v>53</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>54</v>
@@ -1042,7 +1042,7 @@
         <v>55</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>56</v>
@@ -1062,7 +1062,7 @@
         <v>57</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>58</v>
@@ -1085,7 +1085,7 @@
         <v>59</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>60</v>
@@ -1105,7 +1105,7 @@
         <v>61</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
marked items in progress
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
   <si>
     <t xml:space="preserve">PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -55,49 +55,52 @@
     <t xml:space="preserve">H, 1</t>
   </si>
   <si>
+    <t xml:space="preserve">IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← from focus group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to be asked to verify before a schedule is deleted, so that I do not accidently delete a schedule.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the app to automatically determine the geographical location of buildings that my classes are in based only on the name of the building as provided by the schedule in the TTU registration system, so that I can easily have my schedule generated without research or prior knowledge of where the buildings are.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to be presented with a message the first time I load the app that informs me of the privacy implications of using the app, so that I am aware of how my information is being handled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the app to show me the shortest walking route between classes, so that I can arrive as quickly as possible in the event that I am running late.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to be able to arbitrarily add some other locations to the app and to my schedules, so that I can plan in regular lunch destinations or walks for exercise between classes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H, 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the app to intelligently determine when classes for the day are already over and provide the reduced set of directions only to classes which are not yet over, so that I am not encumbered by excess, unnecessary information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undecided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M, 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">← from focus group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be asked to verify before a schedule is deleted, so that I do not accidently delete a schedule.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to automatically determine the geographical location of buildings that my classes are in based only on the name of the building as provided by the schedule in the TTU registration system, so that I can easily have my schedule generated without research or prior knowledge of where the buildings are.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be presented with a message the first time I load the app that informs me of the privacy implications of using the app, so that I am aware of how my information is being handled.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to show me the shortest walking route between classes, so that I can arrive as quickly as possible in the event that I am running late.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to arbitrarily add some other locations to the app and to my schedules, so that I can plan in regular lunch destinations or walks for exercise between classes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to intelligently determine when classes for the day are already over and provide the reduced set of directions only to classes which are not yet over, so that I am not encumbered by excess, unnecessary information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Undecided</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M, 7</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want the app to recalculate the shortest path to the next destination in my schedule with the push of a ‘recalculate’ button, in the event that I veer from the original route and require new directions.</t>
@@ -353,6 +356,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
         <bgColor rgb="FFCE181E"/>
       </patternFill>
@@ -367,12 +376,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF00CC33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -450,32 +453,32 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -567,7 +570,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -675,7 +678,7 @@
       <c r="D10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -695,7 +698,7 @@
       <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="0" t="n">
@@ -755,8 +758,8 @@
       <c r="D14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>11</v>
+      <c r="E14" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>2</v>
@@ -767,16 +770,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>1</v>
@@ -787,16 +790,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>2</v>
@@ -807,16 +810,16 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>3</v>
@@ -827,16 +830,16 @@
         <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>11</v>
+        <v>35</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>5</v>
@@ -847,16 +850,16 @@
         <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>1</v>
@@ -867,16 +870,16 @@
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>2</v>
@@ -887,22 +890,22 @@
         <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>6</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,22 +913,22 @@
         <v>26</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,22 +936,22 @@
         <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>7</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,22 +959,22 @@
         <v>25</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>9</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,16 +982,16 @@
         <v>18</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>4</v>
@@ -999,16 +1002,16 @@
         <v>7</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>11</v>
+        <v>53</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>4</v>
@@ -1019,16 +1022,16 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>2</v>
@@ -1039,16 +1042,16 @@
         <v>17</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>11</v>
+        <v>57</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>4</v>
@@ -1059,16 +1062,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>11</v>
+        <v>59</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>2</v>
@@ -1082,16 +1085,16 @@
         <v>20</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>11</v>
+        <v>61</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>7</v>
@@ -1102,22 +1105,22 @@
         <v>22</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>11</v>
+        <v>63</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>5</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1127,31 +1130,31 @@
       <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>66</v>
+      <c r="E34" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>3</v>
@@ -1162,13 +1165,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>66</v>
+      <c r="E35" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>3</v>
@@ -1179,13 +1182,13 @@
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E36" s="10" t="s">
-        <v>66</v>
+      <c r="E36" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>3</v>
@@ -1196,13 +1199,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E37" s="10" t="s">
-        <v>66</v>
+      <c r="E37" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>2</v>
@@ -1213,13 +1216,13 @@
         <v>29</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>66</v>
+      <c r="E38" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>3</v>
@@ -1233,13 +1236,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E39" s="10" t="s">
-        <v>66</v>
+      <c r="E39" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>3</v>
@@ -1252,34 +1255,34 @@
       <c r="B41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="11" t="s">
-        <v>72</v>
+      <c r="B42" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B43" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="C43" s="6" t="s">
         <v>78</v>
       </c>
+      <c r="D43" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="E43" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added story 33 to backlog
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
   <si>
     <t xml:space="preserve">PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -148,10 +148,16 @@
     <t xml:space="preserve">← from presentation feedback</t>
   </si>
   <si>
+    <t xml:space="preserve">As a user, I want to be able to review the privacy policy/implications statement at any time, preferably from within the settings menu, so that do not have to take special measures to review the statement if I have forgotten its contents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L, 13</t>
+  </si>
+  <si>
     <t xml:space="preserve">As a user, I want the app to collect a minimal amount of private information about me to perform its work, so that I maintain control of my private information.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 13</t>
+    <t xml:space="preserve">L, 14</t>
   </si>
   <si>
     <t xml:space="preserve">← from deliverable 0 feedback</t>
@@ -160,61 +166,61 @@
     <t xml:space="preserve">As a user, I want the ability to share a location with others who do not have the app, so that I can easily communicate an intended location to friends.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 14</t>
+    <t xml:space="preserve">L, 15</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want the app to be secure, so that information collected by the app is not shared with unintended parties.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 15</t>
+    <t xml:space="preserve">L, 16</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want the ability to share a location with another user of the app, so that I can easily communicate an intended location to friends.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 16</t>
+    <t xml:space="preserve">L, 17</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want to be able to mark a class as temporarily canceled for the day, so that I do not receive unnecessary notifications, reminders, or directions for classes I will not be attending that day.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 17</t>
+    <t xml:space="preserve">L, 18</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I also want the app to give me the option to toggle showing the routes to ALL classes for the day regardless of whether they are already over, so that I can show my schedule to others in person.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 18</t>
+    <t xml:space="preserve">L, 19</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want the app to regularly update and display my current location on the navigation map, so that I can more easily follow the directions provided by the app.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 19</t>
+    <t xml:space="preserve">L, 20</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want to be able to add arbitrary locations which will only be considered on that day only, and not saved to the schedule for use on other days, so that I can benefit from the features of the app even with short-term plans without inconveniencing myself by having to remove destinations from the schedule again later.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 20</t>
+    <t xml:space="preserve">L, 21</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want to be able to set date ranges for entered schedules, so past schedules will automatically be removed.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 21</t>
+    <t xml:space="preserve">L, 22</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want to be able to export schedules to other common digital calendar formats, so that I can integrate some benefits from the app with other apps that I use every day.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 22</t>
+    <t xml:space="preserve">L, 23</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want the app to show me the nearest vending machine location at the push of a button, so that I can avoid excessive travel when I am hungry/thirsty.</t>
   </si>
   <si>
-    <t xml:space="preserve">L, 23</t>
+    <t xml:space="preserve">L, 24</t>
   </si>
   <si>
     <t xml:space="preserve">← Arpit’s idea</t>
@@ -567,10 +573,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -920,9 +926,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>26</v>
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="n">
+        <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>42</v>
@@ -930,31 +936,28 @@
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>44</v>
+      <c r="F23" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>24</v>
@@ -962,11 +965,13 @@
       <c r="F24" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>47</v>
@@ -981,15 +986,13 @@
         <v>24</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>44</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>49</v>
@@ -1004,15 +1007,15 @@
         <v>24</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>51</v>
@@ -1027,12 +1030,15 @@
         <v>24</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>53</v>
@@ -1050,9 +1056,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>55</v>
@@ -1067,12 +1073,12 @@
         <v>24</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>57</v>
@@ -1087,12 +1093,12 @@
         <v>24</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>59</v>
@@ -1107,15 +1113,12 @@
         <v>24</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>61</v>
@@ -1130,12 +1133,15 @@
         <v>24</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>63</v>
@@ -1143,62 +1149,65 @@
       <c r="C33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="0" t="s">
         <v>64</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="F33" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G33" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="4"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="G34" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="4"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9"/>
+      <c r="B36" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="B37" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>2</v>
@@ -1210,12 +1219,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>2</v>
@@ -1227,12 +1236,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>2</v>
@@ -1241,38 +1250,35 @@
         <v>10</v>
       </c>
       <c r="F39" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="0" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>10</v>
@@ -1280,42 +1286,62 @@
       <c r="F41" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="4"/>
+      <c r="G41" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>76</v>
-      </c>
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="E45" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="6" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="C46" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="D46" s="6" t="s">
         <v>81</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a story to match SRS
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">← from focus group</t>
   </si>
   <si>
-    <t xml:space="preserve">As a user, I want to be asked to verify before a schedule is deleted, so that I do not accidently delete a schedule.</t>
+    <t xml:space="preserve">As a user, I want to be asked to verify before a schedule or course is deleted, so that I do not accidentally delete a schedule.</t>
   </si>
   <si>
     <t xml:space="preserve">As a user, I want the app to automatically determine the geographical location of buildings that my classes are in based only on the name of the building as provided by the schedule in the TTU registration system, so that I can easily have my schedule generated without research or prior knowledge of where the buildings are.</t>
@@ -576,7 +576,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updated Product Backlog for Sprint 5
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 4" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sprint 5" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="84">
   <si>
     <t xml:space="preserve">PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -575,19 +576,19 @@
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,7 +681,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1347,7 +1348,792 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="37.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="4"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Updated product backlog PDFized Platform doc
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AC291E-5B91-794A-B8BA-23DA9A68CED0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 4" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sprint 5" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sprint 4" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 5" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -23,266 +28,263 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="84">
   <si>
-    <t xml:space="preserve">PRODUCT BACKLOG — DELIVERABLE 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One user story per row. This document must be updated at minimum at the beginning and end of sprints.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keep sorted by priority.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Priority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want a quick-find feature so that I can find the nearest path to a single destination without inputting a schedule.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">← from focus group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be asked to verify before a schedule or course is deleted, so that I do not accidentally delete a schedule.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to automatically determine the geographical location of buildings that my classes are in based only on the name of the building as provided by the schedule in the TTU registration system, so that I can easily have my schedule generated without research or prior knowledge of where the buildings are.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be presented with a message the first time I load the app that informs me of the privacy implications of using the app, so that I am aware of how my information is being handled.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to show me the shortest walking route between classes, so that I can arrive as quickly as possible in the event that I am running late.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to arbitrarily add some other locations to the app and to my schedules, so that I can plan in regular lunch destinations or walks for exercise between classes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to intelligently determine when classes for the day are already over and provide the reduced set of directions only to classes which are not yet over, so that I am not encumbered by excess, unnecessary information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">undecided</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to recalculate the shortest path to the next destination in my schedule with the push of a ‘recalculate’ button, in the event that I veer from the original route and require new directions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to show me an estimated amount of time to travel from my current location to the next destination in my schedule, so that I can react with more urgency if I am in danger of being late.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H, 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to tell me how much time is available until my next class begins, so that I can more easily fit unscheduled activities into my day without calculating myself the amount of time available until class begins.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M, 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to notify me with special messages when I am in danger of being late to class, based on the time the class begins and the travel time necessary to reach the building, so that I can afford to be distracted and do not have to constantly check the app.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M, 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the reminder feature to honor silent mode and notification settings on the mobile device, so that I am not inconvenienced by additional settings.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M, 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to completely disable all reminder features, regardless of phone notification settings on the mobile device, so that I am not bothered by unnecessary reminders when I am confident about my schedule.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M, 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to select times for my courses from a dropdown menu, so that I can easily set the time without error or knowledge about the internal time format for the app.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M, 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to show me shortest paths which include bus routes, so that I can reach very far destinations on campus quickly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">← from presentation feedback</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to review the privacy policy/implications statement at any time, preferably from within the settings menu, so that do not have to take special measures to review the statement if I have forgotten its contents.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to collect a minimal amount of private information about me to perform its work, so that I maintain control of my private information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">← from deliverable 0 feedback</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the ability to share a location with others who do not have the app, so that I can easily communicate an intended location to friends.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to be secure, so that information collected by the app is not shared with unintended parties.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the ability to share a location with another user of the app, so that I can easily communicate an intended location to friends.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to mark a class as temporarily canceled for the day, so that I do not receive unnecessary notifications, reminders, or directions for classes I will not be attending that day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I also want the app to give me the option to toggle showing the routes to ALL classes for the day regardless of whether they are already over, so that I can show my schedule to others in person.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to regularly update and display my current location on the navigation map, so that I can more easily follow the directions provided by the app.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to add arbitrary locations which will only be considered on that day only, and not saved to the schedule for use on other days, so that I can benefit from the features of the app even with short-term plans without inconveniencing myself by having to remove destinations from the schedule again later.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to set date ranges for entered schedules, so past schedules will automatically be removed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to export schedules to other common digital calendar formats, so that I can integrate some benefits from the app with other apps that I use every day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want the app to show me the nearest vending machine location at the push of a button, so that I can avoid excessive travel when I am hungry/thirsty.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L, 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">← Arpit’s idea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPLETED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to add my class schedule (course building, time) for the day to the app, so that I can receive complete and correct walking directions to each building in order from the app.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to save my schedule for the day and give it a name so that I can recall it quickly in the future.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to save and recall multiple schedules, because I may not have the same schedule every day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to easily delete saved schedules, in case my schedule changes or I have progressed to a new term with different classes, so that I am not encumbered by schedules that are no longer relevant.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to name each schedule myself, so that they are customized to my needs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to be able to edit existing/saved schedules to change the buildings and times of each class, so that I can correct for schedule changes and prior input mistakes without creating entirely new schedules.</t>
+    <t>PRODUCT BACKLOG — DELIVERABLE 3</t>
+  </si>
+  <si>
+    <t>One user story per row. This document must be updated at minimum at the beginning and end of sprints.</t>
+  </si>
+  <si>
+    <t>Keep sorted by priority.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Story Priority</t>
+  </si>
+  <si>
+    <t>Story Status</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>As a user, I want a quick-find feature so that I can find the nearest path to a single destination without inputting a schedule.</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>← from focus group</t>
+  </si>
+  <si>
+    <t>As a user, I want to be asked to verify before a schedule or course is deleted, so that I do not accidentally delete a schedule.</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to automatically determine the geographical location of buildings that my classes are in based only on the name of the building as provided by the schedule in the TTU registration system, so that I can easily have my schedule generated without research or prior knowledge of where the buildings are.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be presented with a message the first time I load the app that informs me of the privacy implications of using the app, so that I am aware of how my information is being handled.</t>
+  </si>
+  <si>
+    <t>H, 1</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to show me the shortest walking route between classes, so that I can arrive as quickly as possible in the event that I am running late.</t>
+  </si>
+  <si>
+    <t>H, 2</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to arbitrarily add some other locations to the app and to my schedules, so that I can plan in regular lunch destinations or walks for exercise between classes.</t>
+  </si>
+  <si>
+    <t>H, 3</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to intelligently determine when classes for the day are already over and provide the reduced set of directions only to classes which are not yet over, so that I am not encumbered by excess, unnecessary information.</t>
+  </si>
+  <si>
+    <t>undecided</t>
+  </si>
+  <si>
+    <t>H, 4</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to recalculate the shortest path to the next destination in my schedule with the push of a ‘recalculate’ button, in the event that I veer from the original route and require new directions.</t>
+  </si>
+  <si>
+    <t>H, 5</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to show me an estimated amount of time to travel from my current location to the next destination in my schedule, so that I can react with more urgency if I am in danger of being late.</t>
+  </si>
+  <si>
+    <t>H, 6</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to tell me how much time is available until my next class begins, so that I can more easily fit unscheduled activities into my day without calculating myself the amount of time available until class begins.</t>
+  </si>
+  <si>
+    <t>M, 7</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to notify me with special messages when I am in danger of being late to class, based on the time the class begins and the travel time necessary to reach the building, so that I can afford to be distracted and do not have to constantly check the app.</t>
+  </si>
+  <si>
+    <t>M, 8</t>
+  </si>
+  <si>
+    <t>As a user, I want the reminder feature to honor silent mode and notification settings on the mobile device, so that I am not inconvenienced by additional settings.</t>
+  </si>
+  <si>
+    <t>M, 9</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to completely disable all reminder features, regardless of phone notification settings on the mobile device, so that I am not bothered by unnecessary reminders when I am confident about my schedule.</t>
+  </si>
+  <si>
+    <t>M, 10</t>
+  </si>
+  <si>
+    <t>As a user, I want to select times for my courses from a dropdown menu, so that I can easily set the time without error or knowledge about the internal time format for the app.</t>
+  </si>
+  <si>
+    <t>M, 11</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to show me shortest paths which include bus routes, so that I can reach very far destinations on campus quickly.</t>
+  </si>
+  <si>
+    <t>L, 12</t>
+  </si>
+  <si>
+    <t>← from presentation feedback</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to review the privacy policy/implications statement at any time, preferably from within the settings menu, so that do not have to take special measures to review the statement if I have forgotten its contents.</t>
+  </si>
+  <si>
+    <t>L, 13</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to collect a minimal amount of private information about me to perform its work, so that I maintain control of my private information.</t>
+  </si>
+  <si>
+    <t>L, 14</t>
+  </si>
+  <si>
+    <t>← from deliverable 0 feedback</t>
+  </si>
+  <si>
+    <t>As a user, I want the ability to share a location with others who do not have the app, so that I can easily communicate an intended location to friends.</t>
+  </si>
+  <si>
+    <t>L, 15</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to be secure, so that information collected by the app is not shared with unintended parties.</t>
+  </si>
+  <si>
+    <t>L, 16</t>
+  </si>
+  <si>
+    <t>As a user, I want the ability to share a location with another user of the app, so that I can easily communicate an intended location to friends.</t>
+  </si>
+  <si>
+    <t>L, 17</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to mark a class as temporarily canceled for the day, so that I do not receive unnecessary notifications, reminders, or directions for classes I will not be attending that day.</t>
+  </si>
+  <si>
+    <t>L, 18</t>
+  </si>
+  <si>
+    <t>As a user, I also want the app to give me the option to toggle showing the routes to ALL classes for the day regardless of whether they are already over, so that I can show my schedule to others in person.</t>
+  </si>
+  <si>
+    <t>L, 19</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to regularly update and display my current location on the navigation map, so that I can more easily follow the directions provided by the app.</t>
+  </si>
+  <si>
+    <t>L, 20</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to add arbitrary locations which will only be considered on that day only, and not saved to the schedule for use on other days, so that I can benefit from the features of the app even with short-term plans without inconveniencing myself by having to remove destinations from the schedule again later.</t>
+  </si>
+  <si>
+    <t>L, 21</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to set date ranges for entered schedules, so past schedules will automatically be removed.</t>
+  </si>
+  <si>
+    <t>L, 22</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to export schedules to other common digital calendar formats, so that I can integrate some benefits from the app with other apps that I use every day.</t>
+  </si>
+  <si>
+    <t>L, 23</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to show me the nearest vending machine location at the push of a button, so that I can avoid excessive travel when I am hungry/thirsty.</t>
+  </si>
+  <si>
+    <t>L, 24</t>
+  </si>
+  <si>
+    <t>← Arpit’s idea</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to add my class schedule (course building, time) for the day to the app, so that I can receive complete and correct walking directions to each building in order from the app.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to save my schedule for the day and give it a name so that I can recall it quickly in the future.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to save and recall multiple schedules, because I may not have the same schedule every day.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to easily delete saved schedules, in case my schedule changes or I have progressed to a new term with different classes, so that I am not encumbered by schedules that are no longer relevant.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to name each schedule myself, so that they are customized to my needs.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to edit existing/saved schedules to change the buildings and times of each class, so that I can correct for schedule changes and prior input mistakes without creating entirely new schedules.</t>
   </si>
   <si>
     <t xml:space="preserve">Story Priorities: </t>
   </si>
   <si>
-    <t xml:space="preserve">H (high)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M (medium)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L (low)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Statuses:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W (waiting)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IP (in progress)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T (testing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D (done)</t>
+    <t>H (high)</t>
+  </si>
+  <si>
+    <t>M (medium)</t>
+  </si>
+  <si>
+    <t>L (low)</t>
+  </si>
+  <si>
+    <t>Story Statuses:</t>
+  </si>
+  <si>
+    <t>W (waiting)</t>
+  </si>
+  <si>
+    <t>IP (in progress)</t>
+  </si>
+  <si>
+    <t>T (testing)</t>
+  </si>
+  <si>
+    <t>D (done)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -290,30 +292,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -340,7 +327,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFCE181E"/>
       <name val="Arial"/>
@@ -348,7 +335,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,9 +384,15 @@
         <bgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -407,105 +400,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -564,49 +492,357 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="5.5"/>
+    <col min="2" max="2" width="69"/>
+    <col min="3" max="3" width="11"/>
+    <col min="4" max="4" width="14.5"/>
+    <col min="5" max="5" width="12.33203125"/>
+    <col min="6" max="6" width="11.6640625"/>
+    <col min="7" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -626,126 +862,126 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="3">
         <v>4</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="3">
         <v>6</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>4</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row r="10" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>4</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>4</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="37.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:7" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+    <row r="14" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -754,18 +990,18 @@
       <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -774,18 +1010,18 @@
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A16">
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -794,18 +1030,18 @@
       <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -814,18 +1050,18 @@
       <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+    <row r="18" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+      <c r="A18">
         <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -834,18 +1070,18 @@
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+    <row r="19" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -854,18 +1090,18 @@
       <c r="C19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+    <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A20">
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -874,18 +1110,18 @@
       <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>36</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A21">
         <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -894,18 +1130,18 @@
       <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
         <v>23</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -920,15 +1156,15 @@
       <c r="E22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="3">
         <v>6</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+    <row r="23" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -943,12 +1179,12 @@
       <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A24">
         <v>26</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -957,21 +1193,21 @@
       <c r="C24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>45</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24">
         <v>6</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A25">
         <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -980,19 +1216,19 @@
       <c r="C25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25">
         <v>6</v>
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A26">
         <v>27</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1001,21 +1237,21 @@
       <c r="C26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>50</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26">
         <v>7</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1024,21 +1260,21 @@
       <c r="C27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>52</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27">
         <v>9</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+    <row r="28" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A28">
         <v>18</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -1047,18 +1283,18 @@
       <c r="C28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>54</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+    <row r="29" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A29">
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1067,18 +1303,18 @@
       <c r="C29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" t="s">
         <v>56</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+    <row r="30" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30">
         <v>9</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1087,18 +1323,18 @@
       <c r="C30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" t="s">
         <v>58</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="F30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+      <c r="A31">
         <v>17</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1107,18 +1343,18 @@
       <c r="C31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" t="s">
         <v>60</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31">
         <v>4</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+    <row r="32" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A32">
         <v>28</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1127,21 +1363,21 @@
       <c r="C32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" t="s">
         <v>62</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G32" s="0" t="s">
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+    <row r="33" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+      <c r="A33">
         <v>20</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -1150,18 +1386,18 @@
       <c r="C33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" t="s">
         <v>64</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33">
         <v>7</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+    <row r="34" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34">
         <v>22</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -1176,20 +1412,20 @@
       <c r="E34" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F34" s="3">
         <v>5</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="G34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>68</v>
@@ -1203,132 +1439,132 @@
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+    <row r="37" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37">
         <v>2</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37">
         <v>3</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+    <row r="38" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38">
         <v>2</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+    <row r="39" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39">
         <v>2</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+    <row r="40" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>4</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40">
         <v>2</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="F40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="27" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>29</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41">
         <v>1</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41">
         <v>3</v>
       </c>
-      <c r="G41" s="0" t="s">
+      <c r="G41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+    <row r="42" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>19</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42">
         <v>2</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B45" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" t="s">
         <v>77</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B46" s="12" t="s">
         <v>79</v>
       </c>
@@ -1346,54 +1582,46 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="5.5"/>
+    <col min="2" max="2" width="69"/>
+    <col min="3" max="3" width="11"/>
+    <col min="4" max="4" width="14.5"/>
+    <col min="5" max="5" width="12.33203125"/>
+    <col min="6" max="6" width="11.6640625"/>
+    <col min="7" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1413,68 +1641,68 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8">
         <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="37.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="E10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A11">
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1483,18 +1711,18 @@
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A12">
         <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1503,18 +1731,18 @@
       <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1523,18 +1751,18 @@
       <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1543,18 +1771,18 @@
       <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+      <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1563,18 +1791,18 @@
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="55.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+    <row r="16" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1583,18 +1811,18 @@
       <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1603,18 +1831,18 @@
       <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A18">
         <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1623,18 +1851,18 @@
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+    <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
         <v>23</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1649,15 +1877,15 @@
       <c r="E19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="3">
         <v>6</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+    <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
         <v>33</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1672,12 +1900,12 @@
       <c r="E20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A21">
         <v>26</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1686,21 +1914,21 @@
       <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21">
         <v>6</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A22">
         <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1709,19 +1937,19 @@
       <c r="C22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22">
         <v>6</v>
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A23">
         <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1730,21 +1958,21 @@
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" t="s">
         <v>50</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23">
         <v>7</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A24">
         <v>25</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1753,21 +1981,21 @@
       <c r="C24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>52</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24">
         <v>9</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+    <row r="25" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A25">
         <v>18</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1776,18 +2004,18 @@
       <c r="C25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>54</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+    <row r="26" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A26">
         <v>7</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1796,18 +2024,18 @@
       <c r="C26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>56</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+    <row r="27" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27">
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1816,18 +2044,18 @@
       <c r="C27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="F27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+      <c r="A28">
         <v>17</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -1836,18 +2064,18 @@
       <c r="C28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>60</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+    <row r="29" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1856,21 +2084,21 @@
       <c r="C29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" t="s">
         <v>62</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G29" s="0" t="s">
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+    <row r="30" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A30">
         <v>20</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1879,18 +2107,18 @@
       <c r="C30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" t="s">
         <v>64</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30">
         <v>7</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+    <row r="31" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31">
         <v>22</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1905,20 +2133,20 @@
       <c r="E31" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="3">
         <v>5</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="G31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="10" t="s">
         <v>68</v>
@@ -1932,187 +2160,187 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34">
         <v>2</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34">
         <v>3</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+    <row r="35" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35">
         <v>2</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+    <row r="36" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36">
         <v>2</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+    <row r="37" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>4</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37">
         <v>2</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="27" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>29</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38">
         <v>1</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38">
         <v>3</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="G38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+    <row r="39" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>19</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39">
         <v>2</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="n">
+    <row r="40" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
         <v>24</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="3">
         <v>4</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="3">
         <v>6</v>
       </c>
-      <c r="G40" s="0" t="s">
+      <c r="G40" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+    <row r="41" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>30</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41">
         <v>4</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" s="0" t="s">
+      <c r="G41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+    <row r="42" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>5</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42">
         <v>4</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42">
         <v>4</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B44" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" t="s">
         <v>77</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B45" s="12" t="s">
         <v>79</v>
       </c>
@@ -2129,14 +2357,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
srs and product backlog about us8
update srs and product backlog about us8
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuyon\Documents\GitHub\RaiderNAV\docs\deliverable3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AC291E-5B91-794A-B8BA-23DA9A68CED0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 4" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="85">
   <si>
     <t>PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -278,12 +277,15 @@
   </si>
   <si>
     <t>D (done)</t>
+  </si>
+  <si>
+    <t>As a user, I want the app to show me the shortest walking route between two locations, so that I can arrive as quickly as possible in the event that I am running late.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -432,8 +434,36 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -809,40 +839,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5"/>
+    <col min="1" max="1" width="5.42578125"/>
     <col min="2" max="2" width="69"/>
     <col min="3" max="3" width="11"/>
-    <col min="4" max="4" width="14.5"/>
-    <col min="5" max="5" width="12.33203125"/>
-    <col min="6" max="6" width="11.6640625"/>
-    <col min="7" max="1025" width="8.5"/>
+    <col min="4" max="4" width="14.42578125"/>
+    <col min="5" max="5" width="12.28515625"/>
+    <col min="6" max="6" width="11.7109375"/>
+    <col min="7" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -862,7 +892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>24</v>
       </c>
@@ -883,7 +913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -903,7 +933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -920,7 +950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>21</v>
       </c>
@@ -940,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -960,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
@@ -980,7 +1010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1000,7 +1030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1020,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1040,7 +1070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1060,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1080,7 +1110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1100,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
@@ -1120,7 +1150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>32</v>
       </c>
@@ -1140,7 +1170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>23</v>
       </c>
@@ -1163,7 +1193,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>33</v>
       </c>
@@ -1183,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>26</v>
       </c>
@@ -1206,7 +1236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>31</v>
       </c>
@@ -1227,7 +1257,7 @@
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>27</v>
       </c>
@@ -1250,7 +1280,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1273,7 +1303,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>18</v>
       </c>
@@ -1293,7 +1323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1313,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1333,7 +1363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1353,7 +1383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1376,7 +1406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20</v>
       </c>
@@ -1396,7 +1426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>22</v>
       </c>
@@ -1419,13 +1449,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>68</v>
@@ -1439,7 +1469,7 @@
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1456,7 +1486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1473,7 +1503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1490,7 +1520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1507,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>29</v>
       </c>
@@ -1527,7 +1557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>19</v>
       </c>
@@ -1544,13 +1574,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B45" s="12" t="s">
         <v>75</v>
       </c>
@@ -1564,7 +1594,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B46" s="12" t="s">
         <v>79</v>
       </c>
@@ -1588,40 +1618,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5"/>
+    <col min="1" max="1" width="5.42578125"/>
     <col min="2" max="2" width="69"/>
     <col min="3" max="3" width="11"/>
-    <col min="4" max="4" width="14.5"/>
-    <col min="5" max="5" width="12.33203125"/>
-    <col min="6" max="6" width="11.6640625"/>
-    <col min="7" max="1025" width="8.5"/>
+    <col min="4" max="4" width="14.42578125"/>
+    <col min="5" max="5" width="12.28515625"/>
+    <col min="6" max="6" width="11.7109375"/>
+    <col min="7" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1641,7 +1671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>21</v>
       </c>
@@ -1661,12 +1691,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -1681,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
@@ -1701,7 +1731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1721,7 +1751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>15</v>
       </c>
@@ -1741,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1761,7 +1791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1781,7 +1811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1801,7 +1831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1821,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1841,7 +1871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>32</v>
       </c>
@@ -1861,7 +1891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>23</v>
       </c>
@@ -1884,7 +1914,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>33</v>
       </c>
@@ -1904,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>26</v>
       </c>
@@ -1927,7 +1957,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>31</v>
       </c>
@@ -1948,7 +1978,7 @@
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>27</v>
       </c>
@@ -1971,7 +2001,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>25</v>
       </c>
@@ -1994,7 +2024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>18</v>
       </c>
@@ -2014,7 +2044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7</v>
       </c>
@@ -2034,7 +2064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2054,7 +2084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>17</v>
       </c>
@@ -2074,7 +2104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2097,7 +2127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
@@ -2117,7 +2147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>22</v>
       </c>
@@ -2140,13 +2170,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="10" t="s">
         <v>68</v>
@@ -2160,7 +2190,7 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2177,7 +2207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2194,7 +2224,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2211,7 +2241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2228,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>29</v>
       </c>
@@ -2248,7 +2278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>19</v>
       </c>
@@ -2265,7 +2295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>24</v>
       </c>
@@ -2286,7 +2316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>30</v>
       </c>
@@ -2306,7 +2336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2323,10 +2353,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
         <v>75</v>
       </c>
@@ -2340,7 +2370,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B45" s="12" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Updated Product Backlog. Updated SRS TOC & PDFized
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuyon\Documents\GitHub\RaiderNAV\docs\deliverable3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1420375-C5FC-9A44-983B-195944BE2E51}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="989" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16420" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 4" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="85">
   <si>
     <t>PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -285,7 +286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -337,7 +338,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +393,12 @@
         <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -406,7 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -429,6 +436,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -459,7 +471,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -839,40 +851,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125"/>
+    <col min="1" max="1" width="5.5"/>
     <col min="2" max="2" width="69"/>
     <col min="3" max="3" width="11"/>
-    <col min="4" max="4" width="14.42578125"/>
-    <col min="5" max="5" width="12.28515625"/>
-    <col min="6" max="6" width="11.7109375"/>
-    <col min="7" max="1025" width="8.42578125"/>
+    <col min="4" max="4" width="14.5"/>
+    <col min="5" max="5" width="12.33203125"/>
+    <col min="6" max="6" width="11.6640625"/>
+    <col min="7" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -892,7 +904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>24</v>
       </c>
@@ -913,7 +925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>30</v>
       </c>
@@ -933,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>
       </c>
@@ -950,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>21</v>
       </c>
@@ -970,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="37" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>8</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>16</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1050,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1070,7 +1082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1130,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>14</v>
       </c>
@@ -1150,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>32</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>23</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>33</v>
       </c>
@@ -1213,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>26</v>
       </c>
@@ -1236,7 +1248,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>31</v>
       </c>
@@ -1257,7 +1269,7 @@
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>27</v>
       </c>
@@ -1280,7 +1292,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>18</v>
       </c>
@@ -1323,7 +1335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1363,7 +1375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1383,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1406,7 +1418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>20</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>22</v>
       </c>
@@ -1449,13 +1461,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>68</v>
@@ -1469,7 +1481,7 @@
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1486,7 +1498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1503,7 +1515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1520,7 +1532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1537,7 +1549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="27" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>29</v>
       </c>
@@ -1557,7 +1569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="40" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>19</v>
       </c>
@@ -1574,13 +1586,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B45" s="12" t="s">
         <v>75</v>
       </c>
@@ -1594,7 +1606,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B46" s="12" t="s">
         <v>79</v>
       </c>
@@ -1618,40 +1630,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A9" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125"/>
+    <col min="1" max="1" width="5.5"/>
     <col min="2" max="2" width="69"/>
     <col min="3" max="3" width="11"/>
-    <col min="4" max="4" width="14.42578125"/>
-    <col min="5" max="5" width="12.28515625"/>
-    <col min="6" max="6" width="11.7109375"/>
-    <col min="7" max="1025" width="8.42578125"/>
+    <col min="4" max="4" width="14.5"/>
+    <col min="5" max="5" width="12.33203125"/>
+    <col min="6" max="6" width="11.6640625"/>
+    <col min="7" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1671,391 +1683,391 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A10">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8">
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9">
+    <row r="11" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9">
+    </row>
+    <row r="14" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10">
+    <row r="15" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>32</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="17" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+      <c r="A17" s="3">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="3">
         <v>6</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+      <c r="A19">
         <v>26</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+      <c r="A21">
         <v>27</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>32</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>23</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="3">
-        <v>6</v>
-      </c>
-      <c r="G19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>33</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>26</v>
-      </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F22">
-        <v>6</v>
-      </c>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+      <c r="A24">
         <v>7</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>25</v>
-      </c>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25">
         <v>9</v>
       </c>
-      <c r="G24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>18</v>
-      </c>
       <c r="B25" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="65" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>24</v>
@@ -2064,18 +2076,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>24</v>
@@ -2083,119 +2095,124 @@
       <c r="F27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="3">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="40" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-      <c r="G29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>20</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>22</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="3">
-        <v>5</v>
-      </c>
-      <c r="G31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="4"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
       <c r="B34" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2204,18 +2221,18 @@
         <v>10</v>
       </c>
       <c r="F34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>10</v>
@@ -2223,13 +2240,16 @@
       <c r="F35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2241,149 +2261,125 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="39" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>24</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="3">
         <v>4</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F37" s="3">
+        <v>6</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>24</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>21</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="3">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="3">
-        <v>6</v>
-      </c>
-      <c r="G40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C41">
-        <v>4</v>
-      </c>
-      <c r="E41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>5</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B44" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="12" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B42" s="16"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B43" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E43" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F43" s="14" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed SRS and product backlog issues
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1420375-C5FC-9A44-983B-195944BE2E51}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A595AA6-B5CF-424D-8755-C62B595E1305}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16420" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="89">
   <si>
     <t>PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -281,6 +281,18 @@
   </si>
   <si>
     <t>As a user, I want the app to show me the shortest walking route between two locations, so that I can arrive as quickly as possible in the event that I am running late.</t>
+  </si>
+  <si>
+    <t>M, 5</t>
+  </si>
+  <si>
+    <t>M, 6</t>
+  </si>
+  <si>
+    <t>L, 10</t>
+  </si>
+  <si>
+    <t>L, 11</t>
   </si>
 </sst>
 </file>
@@ -1633,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="106" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A9" sqref="A8:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1694,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>24</v>
@@ -1714,7 +1726,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>24</v>
@@ -1734,7 +1746,7 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>24</v>
@@ -1754,7 +1766,7 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>24</v>
@@ -1774,7 +1786,7 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>24</v>
@@ -1794,7 +1806,7 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>24</v>
@@ -1814,7 +1826,7 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>24</v>
@@ -1834,7 +1846,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>24</v>
@@ -1854,7 +1866,7 @@
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>24</v>
@@ -1874,7 +1886,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>24</v>
@@ -1897,7 +1909,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>24</v>
@@ -1917,7 +1929,7 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>24</v>
@@ -1940,7 +1952,7 @@
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>24</v>
@@ -1961,7 +1973,7 @@
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>24</v>
@@ -1984,7 +1996,7 @@
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>24</v>
@@ -2007,7 +2019,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
@@ -2027,7 +2039,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>24</v>
@@ -2047,7 +2059,7 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>24</v>
@@ -2067,7 +2079,7 @@
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>24</v>
@@ -2087,7 +2099,7 @@
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>24</v>
@@ -2110,7 +2122,7 @@
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>24</v>
@@ -2130,7 +2142,7 @@
         <v>22</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Fixed product backlog issues
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A595AA6-B5CF-424D-8755-C62B595E1305}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47AC7DF-2DB7-6F45-8350-FC77CBA21D3B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16420" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="89">
   <si>
     <t>PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -866,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="B31" zoomScale="125" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1645,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="172" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D41" sqref="D40:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2341,9 +2341,6 @@
       <c r="C40">
         <v>5</v>
       </c>
-      <c r="D40" t="s">
-        <v>15</v>
-      </c>
       <c r="E40" s="18" t="s">
         <v>10</v>
       </c>
@@ -2360,9 +2357,6 @@
       </c>
       <c r="C41">
         <v>5</v>
-      </c>
-      <c r="D41" t="s">
-        <v>18</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Fixed product backlog issue
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47AC7DF-2DB7-6F45-8350-FC77CBA21D3B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E684292-9420-774E-BCD6-60E197524B26}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16420" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="89">
   <si>
     <t>PRODUCT BACKLOG — DELIVERABLE 3</t>
   </si>
@@ -1645,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="172" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D41" sqref="D40:D41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1702,8 +1702,8 @@
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
-        <v>5</v>
+      <c r="C8" t="s">
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
SRS and Product Backlog
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_ProductBacklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C778272-BA22-D54F-BDB2-87EE52E7A04E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5EDDDD-EA0A-5445-8B50-FB492E7B4F47}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 4" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
     <t>As a user, I want the app to show me the shortest walking route between two locations, so that I can arrive as quickly as possible in the event that I am running late.</t>
   </si>
   <si>
-    <t>As a user, I want my information encrypted in transaction so that both the confidentiality and integrity are protected.</t>
+    <t>As a user, I want my information encrypted in transaction so that both the confidentiality and integrity of my transaction are protected.</t>
   </si>
 </sst>
 </file>
@@ -1615,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="167" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="167" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>